<commit_message>
add class & update all
</commit_message>
<xml_diff>
--- a/20191118-Plan-Project-HR-Admin.xlsx
+++ b/20191118-Plan-Project-HR-Admin.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A292D8D-7A85-4CF1-AF16-AB93E8FDBEB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D65905D-678E-4DC2-BEE5-49155E4CE097}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -181,9 +181,6 @@
     <t>2.2 วิเคราะห์ระบบจาก Requirement เพื่อสร้าง Entity</t>
   </si>
   <si>
-    <t>3.1 Design Flow Chart</t>
-  </si>
-  <si>
     <t>3.2 Design Class Diagram</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>3.1 Design Flow Chart , Activity diagram</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1245,7 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1716,9 +1716,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="39" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3135,8 +3132,8 @@
   </sheetPr>
   <dimension ref="A1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3163,7 +3160,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="20"/>
@@ -3188,36 +3185,36 @@
       <c r="G2" s="24"/>
       <c r="H2" s="25"/>
       <c r="I2" s="38"/>
-      <c r="L2" s="188" t="s">
+      <c r="L2" s="187" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="188"/>
-      <c r="N2" s="188"/>
-      <c r="O2" s="188"/>
-      <c r="Q2" s="189" t="s">
+      <c r="M2" s="187"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="187"/>
+      <c r="Q2" s="188" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="189"/>
-      <c r="S2" s="189"/>
-      <c r="T2" s="189"/>
-      <c r="V2" s="190" t="s">
+      <c r="R2" s="188"/>
+      <c r="S2" s="188"/>
+      <c r="T2" s="188"/>
+      <c r="V2" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="190"/>
-      <c r="X2" s="190"/>
-      <c r="Y2" s="190"/>
-      <c r="AA2" s="180" t="s">
+      <c r="W2" s="189"/>
+      <c r="X2" s="189"/>
+      <c r="Y2" s="189"/>
+      <c r="AA2" s="179" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" s="180"/>
-      <c r="AC2" s="180"/>
-      <c r="AD2" s="180"/>
-      <c r="AF2" s="181" t="s">
+      <c r="AB2" s="179"/>
+      <c r="AC2" s="179"/>
+      <c r="AD2" s="179"/>
+      <c r="AF2" s="180" t="s">
         <v>9</v>
       </c>
-      <c r="AG2" s="181"/>
-      <c r="AH2" s="181"/>
-      <c r="AI2" s="181"/>
+      <c r="AG2" s="180"/>
+      <c r="AH2" s="180"/>
+      <c r="AI2" s="180"/>
     </row>
     <row r="3" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -3227,16 +3224,16 @@
         <v>41</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="182" t="s">
+      <c r="D3" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="183"/>
-      <c r="F3" s="185">
+      <c r="E3" s="182"/>
+      <c r="F3" s="184">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start Date])=0,TODAY(),MIN(Milestones[Start Date])),TODAY())</f>
         <v>43789</v>
       </c>
-      <c r="G3" s="186"/>
-      <c r="H3" s="187"/>
+      <c r="G3" s="185"/>
+      <c r="H3" s="186"/>
       <c r="I3" s="34"/>
       <c r="J3" s="33"/>
       <c r="K3" s="36"/>
@@ -3248,10 +3245,10 @@
       <c r="B4" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="182" t="s">
+      <c r="D4" s="181" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="183"/>
+      <c r="E4" s="182"/>
       <c r="F4" s="11">
         <v>0</v>
       </c>
@@ -3341,15 +3338,15 @@
       <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="184"/>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184"/>
+      <c r="B5" s="183"/>
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="183"/>
       <c r="K5" s="36"/>
       <c r="L5" s="15">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
@@ -3651,34 +3648,34 @@
       <c r="A7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="174" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="176" t="s">
+      <c r="C7" s="175" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="176" t="s">
+      <c r="D7" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="176" t="s">
+      <c r="E7" s="175" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="176" t="s">
+      <c r="F7" s="175" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="176" t="s">
+      <c r="G7" s="175" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="176" t="s">
+      <c r="H7" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="177" t="s">
+      <c r="I7" s="176" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="178" t="s">
+      <c r="J7" s="177" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="179" t="s">
+      <c r="K7" s="178" t="s">
         <v>32</v>
       </c>
       <c r="L7" s="9" t="str">
@@ -3926,8 +3923,8 @@
         <f>H9</f>
         <v>1</v>
       </c>
-      <c r="I8" s="174"/>
-      <c r="J8" s="160"/>
+      <c r="I8" s="173"/>
+      <c r="J8" s="159"/>
       <c r="K8" s="55"/>
       <c r="L8" s="35" t="str">
         <f t="shared" ref="L8:U12" ca="1" si="6">IF(AND($C8="Goal",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1),2,IF(AND($C8="Milestone",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1),1,""))</f>
@@ -4156,19 +4153,19 @@
     </row>
     <row r="9" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
-      <c r="B9" s="170" t="s">
-        <v>53</v>
+      <c r="B9" s="169" t="s">
+        <v>52</v>
       </c>
       <c r="C9" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="125" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="171">
+        <v>51</v>
+      </c>
+      <c r="E9" s="170">
         <v>1</v>
       </c>
-      <c r="F9" s="172">
+      <c r="F9" s="171">
         <v>43789</v>
       </c>
       <c r="G9" s="99">
@@ -4178,7 +4175,7 @@
         <f>Milestones[[#This Row],[End Date]]-Milestones[[#This Row],[Start Date]]</f>
         <v>1</v>
       </c>
-      <c r="I9" s="173">
+      <c r="I9" s="172">
         <v>43789</v>
       </c>
       <c r="J9" s="88">
@@ -4420,20 +4417,20 @@
       </c>
       <c r="C10" s="76"/>
       <c r="D10" s="81"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="166">
+      <c r="E10" s="164"/>
+      <c r="F10" s="165">
         <f>F11</f>
         <v>43790</v>
       </c>
-      <c r="G10" s="167">
+      <c r="G10" s="166">
         <f>G12</f>
         <v>43791</v>
       </c>
-      <c r="H10" s="168">
+      <c r="H10" s="167">
         <f>H11+H12</f>
         <v>2</v>
       </c>
-      <c r="I10" s="169"/>
+      <c r="I10" s="168"/>
       <c r="J10" s="147"/>
       <c r="K10" s="46"/>
       <c r="L10" s="35" t="str">
@@ -4670,7 +4667,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="133">
         <v>1</v>
@@ -4930,7 +4927,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="69">
         <v>1</v>
@@ -5200,7 +5197,7 @@
         <v>9</v>
       </c>
       <c r="I13" s="54"/>
-      <c r="J13" s="160"/>
+      <c r="J13" s="159"/>
       <c r="K13" s="55"/>
       <c r="L13" s="35"/>
       <c r="M13" s="10"/>
@@ -5262,16 +5259,16 @@
     <row r="14" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="127" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C14" s="73" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="78" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="62">
         <f>G12</f>
@@ -5284,14 +5281,16 @@
       <c r="H14" s="126">
         <v>3</v>
       </c>
-      <c r="I14" s="159"/>
+      <c r="I14" s="92">
+        <v>43794</v>
+      </c>
       <c r="J14" s="87">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I14-Milestones[[#This Row],[End Date]])</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K14" s="49" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I14-G14&gt;0,"Delay","Complete"))),"Complete")</f>
-        <v>On Process</v>
+        <v>Complete</v>
       </c>
       <c r="L14" s="35"/>
       <c r="M14" s="10"/>
@@ -5353,16 +5352,16 @@
     <row r="15" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="43"/>
       <c r="B15" s="58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="72" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="69">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F15" s="66">
         <f>G14</f>
@@ -5375,14 +5374,16 @@
       <c r="H15" s="59">
         <v>3</v>
       </c>
-      <c r="I15" s="118"/>
+      <c r="I15" s="118">
+        <v>43797</v>
+      </c>
       <c r="J15" s="91">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I15-Milestones[[#This Row],[End Date]])</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K15" s="57" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I15-G15&gt;0,"Delay","Complete"))),"Complete")</f>
-        <v>On Process</v>
+        <v>Complete</v>
       </c>
       <c r="L15" s="35"/>
       <c r="M15" s="10"/>
@@ -5443,15 +5444,15 @@
     </row>
     <row r="16" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="43"/>
-      <c r="B16" s="163" t="s">
-        <v>46</v>
+      <c r="B16" s="162" t="s">
+        <v>45</v>
       </c>
       <c r="C16" s="42"/>
       <c r="D16" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="70">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="62">
         <f>G15</f>
@@ -5464,14 +5465,16 @@
       <c r="H16" s="126">
         <v>3</v>
       </c>
-      <c r="I16" s="92"/>
+      <c r="I16" s="92">
+        <v>43800</v>
+      </c>
       <c r="J16" s="87">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I16-Milestones[[#This Row],[End Date]])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="49" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I16-G16&gt;0,"Delay","Complete"))),"Complete")</f>
-        <v>On Process</v>
+        <v>Complete</v>
       </c>
       <c r="L16" s="35"/>
       <c r="M16" s="10"/>
@@ -5531,13 +5534,13 @@
       <c r="BO16" s="10"/>
     </row>
     <row r="17" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="164" t="s">
+      <c r="B17" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="162"/>
+      <c r="C17" s="161"/>
       <c r="D17" s="103"/>
       <c r="E17" s="151"/>
-      <c r="F17" s="161">
+      <c r="F17" s="160">
         <f>G16</f>
         <v>43800</v>
       </c>
@@ -5780,11 +5783,11 @@
     <row r="18" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="43"/>
       <c r="B18" s="109" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="108"/>
       <c r="D18" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="69">
         <v>0.5</v>
@@ -5803,7 +5806,7 @@
       <c r="I18" s="110"/>
       <c r="J18" s="94">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I18-Milestones[[#This Row],[End Date]])</f>
-        <v>-4</v>
+        <v>3</v>
       </c>
       <c r="K18" s="87" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I18-G18&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -5869,16 +5872,16 @@
     <row r="19" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="43"/>
       <c r="B19" s="106" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="73" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="78" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="70">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F19" s="118">
         <f>G18</f>
@@ -5894,11 +5897,11 @@
       <c r="I19" s="62"/>
       <c r="J19" s="49">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I19-Milestones[[#This Row],[End Date]])</f>
-        <v>-9</v>
+        <v>-2</v>
       </c>
       <c r="K19" s="87" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I19-G19&gt;0,"Delay","Complete"))),"Complete")</f>
-        <v>Pending</v>
+        <v>On Process</v>
       </c>
       <c r="L19" s="35"/>
       <c r="M19" s="10"/>
@@ -5960,14 +5963,14 @@
     <row r="20" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="43"/>
       <c r="B20" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="72"/>
       <c r="D20" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="115">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F20" s="118">
         <f t="shared" ref="F20:F27" si="14">G19</f>
@@ -5980,14 +5983,16 @@
       <c r="H20" s="95">
         <v>5</v>
       </c>
-      <c r="I20" s="63"/>
+      <c r="I20" s="63">
+        <v>43808</v>
+      </c>
       <c r="J20" s="56">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I20-Milestones[[#This Row],[End Date]])</f>
-        <v>-14</v>
+        <v>-7</v>
       </c>
       <c r="K20" s="87" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I20-G20&gt;0,"Delay","Complete"))),"Complete")</f>
-        <v>Pending</v>
+        <v>Complete</v>
       </c>
       <c r="L20" s="35"/>
       <c r="M20" s="10"/>
@@ -6049,11 +6054,11 @@
     <row r="21" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="43"/>
       <c r="B21" s="107" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="73"/>
       <c r="D21" s="78" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="117">
         <v>0.5</v>
@@ -6072,7 +6077,7 @@
       <c r="I21" s="65"/>
       <c r="J21" s="56">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I21-Milestones[[#This Row],[End Date]])</f>
-        <v>-19</v>
+        <v>-12</v>
       </c>
       <c r="K21" s="87" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I21-G21&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6138,11 +6143,11 @@
     <row r="22" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="43"/>
       <c r="B22" s="107" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="104"/>
       <c r="D22" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="70">
         <v>0</v>
@@ -6161,7 +6166,7 @@
       <c r="I22" s="62"/>
       <c r="J22" s="82">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I22-Milestones[[#This Row],[End Date]])</f>
-        <v>-24</v>
+        <v>-17</v>
       </c>
       <c r="K22" s="87" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I22-G22&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6227,11 +6232,11 @@
     <row r="23" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="43"/>
       <c r="B23" s="109" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="70">
         <v>0</v>
@@ -6250,7 +6255,7 @@
       <c r="I23" s="66"/>
       <c r="J23" s="56">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I23-Milestones[[#This Row],[End Date]])</f>
-        <v>-29</v>
+        <v>-22</v>
       </c>
       <c r="K23" s="91" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I23-G23&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6316,11 +6321,11 @@
     <row r="24" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="43"/>
       <c r="B24" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="72"/>
       <c r="D24" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="69">
         <v>0</v>
@@ -6339,7 +6344,7 @@
       <c r="I24" s="62"/>
       <c r="J24" s="57">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I24-Milestones[[#This Row],[End Date]])</f>
-        <v>-34</v>
+        <v>-27</v>
       </c>
       <c r="K24" s="87" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I24-G24&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6405,11 +6410,11 @@
     <row r="25" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="43"/>
       <c r="B25" s="107" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="72"/>
       <c r="D25" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="70">
         <v>0</v>
@@ -6428,7 +6433,7 @@
       <c r="I25" s="66"/>
       <c r="J25" s="57">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I25-Milestones[[#This Row],[End Date]])</f>
-        <v>-39</v>
+        <v>-32</v>
       </c>
       <c r="K25" s="87" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I25-G25&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6493,11 +6498,11 @@
     </row>
     <row r="26" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="109" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="73"/>
       <c r="D26" s="102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="68">
         <v>0</v>
@@ -6516,7 +6521,7 @@
       <c r="I26" s="62"/>
       <c r="J26" s="49">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I26-Milestones[[#This Row],[End Date]])</f>
-        <v>-44</v>
+        <v>-37</v>
       </c>
       <c r="K26" s="87" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I26-G26&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6582,11 +6587,11 @@
     <row r="27" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
       <c r="B27" s="41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="129"/>
       <c r="D27" s="80" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="67">
         <v>0</v>
@@ -6605,7 +6610,7 @@
       <c r="I27" s="61"/>
       <c r="J27" s="130">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I27-Milestones[[#This Row],[End Date]])</f>
-        <v>-49</v>
+        <v>-42</v>
       </c>
       <c r="K27" s="90" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I27-G27&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6689,7 +6694,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="136" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J28" s="137"/>
       <c r="K28" s="137"/>
@@ -6753,13 +6758,13 @@
     <row r="29" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="43"/>
       <c r="B29" s="153" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="129" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="101" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="115">
         <v>0</v>
@@ -6778,7 +6783,7 @@
       <c r="I29" s="154"/>
       <c r="J29" s="155">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I29-Milestones[[#This Row],[End Date]])</f>
-        <v>-55</v>
+        <v>-48</v>
       </c>
       <c r="K29" s="155" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I29-G29&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6924,13 +6929,13 @@
     <row r="31" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="43"/>
       <c r="B31" s="127" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="73" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="78" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" s="70">
         <v>0</v>
@@ -6949,7 +6954,7 @@
       <c r="I31" s="148"/>
       <c r="J31" s="87">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I31-Milestones[[#This Row],[End Date]])</f>
-        <v>-61</v>
+        <v>-54</v>
       </c>
       <c r="K31" s="87" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I31-G31&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7094,13 +7099,13 @@
     </row>
     <row r="33" spans="2:67" ht="15" x14ac:dyDescent="0.25">
       <c r="B33" s="58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="69">
         <v>0</v>
@@ -7119,7 +7124,7 @@
       <c r="I33" s="143"/>
       <c r="J33" s="91">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I33-Milestones[[#This Row],[End Date]])</f>
-        <v>-67</v>
+        <v>-60</v>
       </c>
       <c r="K33" s="91" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I33-G33&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7263,13 +7268,13 @@
     </row>
     <row r="35" spans="2:67" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" s="58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D35" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" s="69">
         <v>0</v>
@@ -7288,7 +7293,7 @@
       <c r="I35" s="143"/>
       <c r="J35" s="91">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I35-Milestones[[#This Row],[End Date]])</f>
-        <v>-72</v>
+        <v>-65</v>
       </c>
       <c r="K35" s="91" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I35-G35&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7434,13 +7439,13 @@
     </row>
     <row r="37" spans="2:67" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" s="105" t="s">
         <v>4</v>
       </c>
       <c r="D37" s="102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37" s="133">
         <v>0</v>
@@ -7459,7 +7464,7 @@
       <c r="I37" s="134"/>
       <c r="J37" s="89">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I37-Milestones[[#This Row],[End Date]])</f>
-        <v>-79</v>
+        <v>-72</v>
       </c>
       <c r="K37" s="89" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I37-G37&gt;0,"Delay","Complete"))),"Complete")</f>

</xml_diff>

<commit_message>
data attendance , approve all 8/01/2020
</commit_message>
<xml_diff>
--- a/20191118-Plan-Project-HR-Admin.xlsx
+++ b/20191118-Plan-Project-HR-Admin.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA2BF58-8923-4602-B468-2DE083D0CA0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE23313-8D52-45A2-82A3-9B2E78769206}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>About This Template</t>
   </si>
@@ -226,9 +226,6 @@
     <t>4.1.1 Login</t>
   </si>
   <si>
-    <t>4.1.2 Employee master</t>
-  </si>
-  <si>
     <t>4.1.3 New employee</t>
   </si>
   <si>
@@ -241,25 +238,85 @@
     <t>4.2 Attendance</t>
   </si>
   <si>
-    <t>4.2.1 Attendance</t>
-  </si>
-  <si>
-    <t>4.2.3 Approve by supervisor</t>
-  </si>
-  <si>
-    <t>4.2.4 Approve by manager</t>
-  </si>
-  <si>
-    <t>4.2.2 Date attendance</t>
-  </si>
-  <si>
     <t>4.1.6 Edit personal information</t>
   </si>
   <si>
     <t>4.1.7 Backup employee master</t>
   </si>
   <si>
-    <t>เหลือ import export</t>
+    <r>
+      <t xml:space="preserve">4.1.2 Employee master                            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">       *เหลือ import export</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.2.1 Attendance                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*เหลือ การลาแบบไม่เต็มวัน</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.2.2 Date attendance                  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*เหลือ filter and  exportData</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.2.3 Approve by supervisor                                   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  *เหลือ filter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.2.4 Approve by manager  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                       *เหลือ filter</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -271,7 +328,7 @@
     <numFmt numFmtId="165" formatCode="d"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +491,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1037,7 +1108,7 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1476,6 +1547,24 @@
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="31" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="31" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="34" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1507,12 +1596,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="31" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1531,6 +1614,272 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="72">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2471,272 +2820,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <sz val="10"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3047,20 +3130,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Milestones" displayName="Milestones" ref="B7:K41" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Milestones" displayName="Milestones" ref="B7:K41" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task Name" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Priority" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="%Progress" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start Date" dataDxfId="52" dataCellStyle="Date"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="End Date" dataDxfId="51" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Durations" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complete Date" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Delay" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task Name" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Priority" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="%Progress" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start Date" dataDxfId="5" dataCellStyle="Date"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="End Date" dataDxfId="4" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Durations" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complete Date" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Delay" dataDxfId="1">
       <calculatedColumnFormula>IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I8-Milestones[[#This Row],[End Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{95D18194-25A8-4EDA-B381-D3500AC79722}" name="Status" dataDxfId="47">
+    <tableColumn id="11" xr3:uid="{95D18194-25A8-4EDA-B381-D3500AC79722}" name="Status" dataDxfId="0">
       <calculatedColumnFormula>IF(Today=Milestones[[#This Row],[Start Date]],"On Process",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process","Complete")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3341,8 +3424,8 @@
   </sheetPr>
   <dimension ref="A1:BO43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3356,7 +3439,7 @@
     <col min="7" max="7" width="9.140625" style="29" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="67" width="3.5703125" style="1" customWidth="1"/>
     <col min="68" max="71" width="8.7109375" style="1"/>
@@ -3394,36 +3477,36 @@
       <c r="G2" s="24"/>
       <c r="H2" s="25"/>
       <c r="I2" s="38"/>
-      <c r="L2" s="156" t="s">
+      <c r="L2" s="162" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="156"/>
-      <c r="N2" s="156"/>
-      <c r="O2" s="156"/>
-      <c r="Q2" s="157" t="s">
+      <c r="M2" s="162"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="Q2" s="163" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="157"/>
-      <c r="S2" s="157"/>
-      <c r="T2" s="157"/>
-      <c r="V2" s="158" t="s">
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
+      <c r="V2" s="164" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="158"/>
-      <c r="X2" s="158"/>
-      <c r="Y2" s="158"/>
-      <c r="AA2" s="148" t="s">
+      <c r="W2" s="164"/>
+      <c r="X2" s="164"/>
+      <c r="Y2" s="164"/>
+      <c r="AA2" s="154" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" s="148"/>
-      <c r="AC2" s="148"/>
-      <c r="AD2" s="148"/>
-      <c r="AF2" s="149" t="s">
+      <c r="AB2" s="154"/>
+      <c r="AC2" s="154"/>
+      <c r="AD2" s="154"/>
+      <c r="AF2" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="AG2" s="149"/>
-      <c r="AH2" s="149"/>
-      <c r="AI2" s="149"/>
+      <c r="AG2" s="155"/>
+      <c r="AH2" s="155"/>
+      <c r="AI2" s="155"/>
     </row>
     <row r="3" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -3433,15 +3516,15 @@
         <v>40</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="150" t="s">
+      <c r="D3" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="151"/>
-      <c r="F3" s="153">
+      <c r="E3" s="157"/>
+      <c r="F3" s="159">
         <v>43789</v>
       </c>
-      <c r="G3" s="154"/>
-      <c r="H3" s="155"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="161"/>
       <c r="I3" s="34"/>
       <c r="J3" s="33"/>
       <c r="K3" s="36"/>
@@ -3453,10 +3536,10 @@
       <c r="B4" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="150" t="s">
+      <c r="D4" s="156" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="151"/>
+      <c r="E4" s="157"/>
       <c r="F4" s="11">
         <v>0</v>
       </c>
@@ -3546,15 +3629,15 @@
       <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="152"/>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
-      <c r="I5" s="152"/>
-      <c r="J5" s="152"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="158"/>
+      <c r="G5" s="158"/>
+      <c r="H5" s="158"/>
+      <c r="I5" s="158"/>
+      <c r="J5" s="158"/>
       <c r="K5" s="36"/>
       <c r="L5" s="15">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
@@ -6082,7 +6165,7 @@
       <c r="H19" s="73">
         <v>5</v>
       </c>
-      <c r="I19" s="132">
+      <c r="I19" s="150">
         <v>43812</v>
       </c>
       <c r="J19" s="133">
@@ -6093,7 +6176,7 @@
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I19-G19&gt;0,"Delay","Complete"))),"Complete")</f>
         <v>Complete</v>
       </c>
-      <c r="L19" s="35"/>
+      <c r="L19" s="108"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
@@ -6150,10 +6233,10 @@
       <c r="BN19" s="10"/>
       <c r="BO19" s="10"/>
     </row>
-    <row r="20" spans="1:67" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="78" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C20" s="65" t="s">
         <v>6</v>
@@ -6165,7 +6248,7 @@
         <v>0.9</v>
       </c>
       <c r="F20" s="84">
-        <f>G19</f>
+        <f t="shared" ref="F20:F25" si="14">G19</f>
         <v>43805</v>
       </c>
       <c r="G20" s="84">
@@ -6175,18 +6258,16 @@
       <c r="H20" s="73">
         <v>5</v>
       </c>
-      <c r="I20" s="132" t="s">
-        <v>70</v>
-      </c>
-      <c r="J20" s="71" t="e">
-        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I20-Milestones[[#This Row],[End Date]])</f>
-        <v>#VALUE!</v>
+      <c r="I20" s="151"/>
+      <c r="J20" s="71">
+        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],L20-Milestones[[#This Row],[End Date]])</f>
+        <v>28</v>
       </c>
       <c r="K20" s="71" t="str">
-        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I20-G20&gt;0,"Delay","Complete"))),"Complete")</f>
-        <v>Complete</v>
-      </c>
-      <c r="L20" s="35"/>
+        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(L20-G20&gt;0,"Delay","Complete"))),"Complete")</f>
+        <v>On Process</v>
+      </c>
+      <c r="L20" s="152"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
@@ -6246,7 +6327,7 @@
     <row r="21" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
       <c r="B21" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="65"/>
       <c r="D21" s="65" t="s">
@@ -6256,7 +6337,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="84">
-        <f>G20</f>
+        <f t="shared" si="14"/>
         <v>43810</v>
       </c>
       <c r="G21" s="84">
@@ -6277,7 +6358,7 @@
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I21-G21&gt;0,"Delay","Complete"))),"Complete")</f>
         <v>Complete</v>
       </c>
-      <c r="L21" s="35"/>
+      <c r="L21" s="108"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
@@ -6337,7 +6418,7 @@
     <row r="22" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="65"/>
       <c r="D22" s="65" t="s">
@@ -6347,7 +6428,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="84">
-        <f>G21</f>
+        <f t="shared" si="14"/>
         <v>43815</v>
       </c>
       <c r="G22" s="84">
@@ -6428,7 +6509,7 @@
     <row r="23" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
       <c r="B23" s="78" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="65"/>
       <c r="D23" s="65" t="s">
@@ -6438,7 +6519,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="84">
-        <f>G22</f>
+        <f t="shared" si="14"/>
         <v>43820</v>
       </c>
       <c r="G23" s="84">
@@ -6519,27 +6600,27 @@
     <row r="24" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="44"/>
       <c r="B24" s="111" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C24" s="76"/>
       <c r="D24" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="159">
+      <c r="E24" s="148">
         <v>1</v>
       </c>
-      <c r="F24" s="160">
-        <f>G23</f>
+      <c r="F24" s="149">
+        <f t="shared" si="14"/>
         <v>43821</v>
       </c>
-      <c r="G24" s="160">
+      <c r="G24" s="149">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
         <v>43822</v>
       </c>
       <c r="H24" s="82">
         <v>1</v>
       </c>
-      <c r="I24" s="160">
+      <c r="I24" s="149">
         <v>43834</v>
       </c>
       <c r="J24" s="106">
@@ -6610,34 +6691,36 @@
     <row r="25" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="78" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C25" s="65"/>
       <c r="D25" s="76" t="s">
         <v>54</v>
       </c>
       <c r="E25" s="83">
-        <v>0</v>
-      </c>
-      <c r="F25" s="160">
-        <f>G24</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="84">
+        <f t="shared" si="14"/>
         <v>43822</v>
       </c>
-      <c r="G25" s="160">
+      <c r="G25" s="84">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
         <v>43823</v>
       </c>
       <c r="H25" s="73">
         <v>1</v>
       </c>
-      <c r="I25" s="84"/>
+      <c r="I25" s="84">
+        <v>43835</v>
+      </c>
       <c r="J25" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I25-Milestones[[#This Row],[End Date]])</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K25" s="71" t="str">
         <f ca="1">IF(Today=Milestones[[#This Row],[Start Date]],"On Process",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process","Complete")))</f>
-        <v>On Process</v>
+        <v>Complete</v>
       </c>
       <c r="L25" s="35"/>
       <c r="M25" s="10"/>
@@ -6699,10 +6782,10 @@
     <row r="26" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
       <c r="B26" s="135" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="136"/>
-      <c r="D26" s="136"/>
+      <c r="D26" s="153"/>
       <c r="E26" s="137"/>
       <c r="F26" s="138"/>
       <c r="G26" s="139"/>
@@ -6767,10 +6850,10 @@
       <c r="BN26" s="10"/>
       <c r="BO26" s="10"/>
     </row>
-    <row r="27" spans="1:67" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="78" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C27" s="65"/>
       <c r="D27" s="65" t="s">
@@ -6793,7 +6876,7 @@
       <c r="I27" s="84"/>
       <c r="J27" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I27-Milestones[[#This Row],[End Date]])</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K27" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I27-G27&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6866,10 +6949,10 @@
         <v>54</v>
       </c>
       <c r="E28" s="83">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="F28" s="84">
-        <f t="shared" ref="F28:F30" si="14">G27</f>
+        <f t="shared" ref="F28:F30" si="15">G27</f>
         <v>43828</v>
       </c>
       <c r="G28" s="84">
@@ -6882,7 +6965,7 @@
       <c r="I28" s="84"/>
       <c r="J28" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I28-Milestones[[#This Row],[End Date]])</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K28" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I28-G28&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6947,7 +7030,7 @@
     </row>
     <row r="29" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="78" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C29" s="65"/>
       <c r="D29" s="65" t="s">
@@ -6957,7 +7040,7 @@
         <v>0.9</v>
       </c>
       <c r="F29" s="84">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>43833</v>
       </c>
       <c r="G29" s="84">
@@ -6970,7 +7053,7 @@
       <c r="I29" s="84"/>
       <c r="J29" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I29-Milestones[[#This Row],[End Date]])</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="K29" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I29-G29&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7035,7 +7118,7 @@
     </row>
     <row r="30" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="78" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C30" s="65"/>
       <c r="D30" s="65" t="s">
@@ -7045,7 +7128,7 @@
         <v>0.9</v>
       </c>
       <c r="F30" s="84">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>43838</v>
       </c>
       <c r="G30" s="84">
@@ -7058,11 +7141,11 @@
       <c r="I30" s="84"/>
       <c r="J30" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I30-Milestones[[#This Row],[End Date]])</f>
-        <v>-9</v>
+        <v>-5</v>
       </c>
       <c r="K30" s="71" t="str">
         <f ca="1">IF(Today=Milestones[[#This Row],[Start Date]],"On Process",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process","Complete")))</f>
-        <v>Pending</v>
+        <v>On Process</v>
       </c>
       <c r="L30" s="35"/>
       <c r="M30" s="35"/>
@@ -7231,7 +7314,7 @@
       <c r="I32" s="105"/>
       <c r="J32" s="106">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I32-Milestones[[#This Row],[End Date]])</f>
-        <v>-15</v>
+        <v>-11</v>
       </c>
       <c r="K32" s="106" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I32-G32&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7401,7 +7484,7 @@
       <c r="I34" s="99"/>
       <c r="J34" s="70">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I34-Milestones[[#This Row],[End Date]])</f>
-        <v>-21</v>
+        <v>-17</v>
       </c>
       <c r="K34" s="70" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I34-G34&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7570,7 +7653,7 @@
       <c r="I36" s="94"/>
       <c r="J36" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I36-Milestones[[#This Row],[End Date]])</f>
-        <v>-27</v>
+        <v>-23</v>
       </c>
       <c r="K36" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I36-G36&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7739,7 +7822,7 @@
       <c r="I38" s="94"/>
       <c r="J38" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I38-Milestones[[#This Row],[End Date]])</f>
-        <v>-32</v>
+        <v>-28</v>
       </c>
       <c r="K38" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I38-G38&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7910,7 +7993,7 @@
       <c r="I40" s="94"/>
       <c r="J40" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I40-Milestones[[#This Row],[End Date]])</f>
-        <v>-39</v>
+        <v>-35</v>
       </c>
       <c r="K40" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I40-G40&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7998,7 +8081,7 @@
       <c r="I41" s="99"/>
       <c r="J41" s="70">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I41-Milestones[[#This Row],[End Date]])</f>
-        <v>-46</v>
+        <v>-42</v>
       </c>
       <c r="K41" s="70" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I41-G41&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -8094,39 +8177,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:BO8 L10:BO11 L35:BO37 L13:BO13 L17:BO20 L31:BO32">
-    <cfRule type="expression" dxfId="46" priority="153">
+    <cfRule type="expression" dxfId="59" priority="153">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:AP4">
-    <cfRule type="expression" dxfId="45" priority="159">
+    <cfRule type="expression" dxfId="58" priority="159">
       <formula>L$5&lt;=EOMONTH($L$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:BO4">
-    <cfRule type="expression" dxfId="44" priority="155">
+    <cfRule type="expression" dxfId="57" priority="155">
       <formula>AND(M$5&lt;=EOMONTH($L$5,2),M$5&gt;EOMONTH($L$5,0),M$5&gt;EOMONTH($L$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:BO4">
-    <cfRule type="expression" dxfId="43" priority="154">
+    <cfRule type="expression" dxfId="56" priority="154">
       <formula>AND(L$5&lt;=EOMONTH($L$5,1),L$5&gt;EOMONTH($L$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:BO17">
-    <cfRule type="expression" dxfId="42" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="176" stopIfTrue="1">
       <formula>AND($C8="Low Risk",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="195" stopIfTrue="1">
       <formula>AND($C8="High Risk",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="213" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="213" stopIfTrue="1">
       <formula>AND($C8="On Track",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="214" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="214" stopIfTrue="1">
       <formula>AND($C8="Med Risk",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="215" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="215" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8145,7 +8228,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:BO12">
-    <cfRule type="expression" dxfId="37" priority="128">
+    <cfRule type="expression" dxfId="50" priority="128">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8164,12 +8247,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:BO9">
-    <cfRule type="expression" dxfId="36" priority="120">
+    <cfRule type="expression" dxfId="49" priority="120">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L34:BO37">
-    <cfRule type="expression" dxfId="35" priority="64">
+    <cfRule type="expression" dxfId="48" priority="64">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8188,22 +8271,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:BO38">
-    <cfRule type="expression" dxfId="34" priority="56">
+    <cfRule type="expression" dxfId="47" priority="56">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:BO38">
-    <cfRule type="expression" dxfId="33" priority="54">
+    <cfRule type="expression" dxfId="46" priority="54">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:BO30">
-    <cfRule type="expression" dxfId="32" priority="43">
+    <cfRule type="expression" dxfId="45" priority="43">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:BO15">
-    <cfRule type="expression" dxfId="31" priority="33">
+    <cfRule type="expression" dxfId="44" priority="33">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8222,7 +8305,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:BO16 L14:BO14">
-    <cfRule type="expression" dxfId="30" priority="35">
+    <cfRule type="expression" dxfId="43" priority="35">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8311,112 +8394,112 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33:BO33">
-    <cfRule type="expression" dxfId="29" priority="18">
+    <cfRule type="expression" dxfId="42" priority="18">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18:BO21">
-    <cfRule type="expression" dxfId="28" priority="409" stopIfTrue="1">
+  <conditionalFormatting sqref="L18:BO19 L21:BO21 M20:BO20">
+    <cfRule type="expression" dxfId="41" priority="409" stopIfTrue="1">
       <formula>AND($C19="Low Risk",L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="410" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="410" stopIfTrue="1">
       <formula>AND($C19="High Risk",L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="411" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="411" stopIfTrue="1">
       <formula>AND($C19="On Track",L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="412" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="412" stopIfTrue="1">
       <formula>AND($C19="Med Risk",L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="413" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="413" stopIfTrue="1">
       <formula>AND(LEN($C19)=0,L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:BO27 L31:BO38">
-    <cfRule type="expression" dxfId="23" priority="421" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="421" stopIfTrue="1">
       <formula>AND($C28="Low Risk",L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="422" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="422" stopIfTrue="1">
       <formula>AND($C28="High Risk",L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="423" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="423" stopIfTrue="1">
       <formula>AND($C28="On Track",L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="424" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="424" stopIfTrue="1">
       <formula>AND($C28="Med Risk",L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="425" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="425" stopIfTrue="1">
       <formula>AND(LEN($C28)=0,L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28:BO30">
-    <cfRule type="expression" dxfId="18" priority="445" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="445" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="446" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="446" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="447" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="447" stopIfTrue="1">
       <formula>AND(#REF!="On Track",L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="448" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="448" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="449" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="449" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39:BO39">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="26" priority="11">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39:BO39">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="25" priority="10">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L40:BO41">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L40:BO41">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39:BO41">
-    <cfRule type="expression" dxfId="9" priority="451" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="451" stopIfTrue="1">
       <formula>AND($C42="Low Risk",L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="452" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="452" stopIfTrue="1">
       <formula>AND($C42="High Risk",L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="453" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="453" stopIfTrue="1">
       <formula>AND($C42="On Track",L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="454" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="454" stopIfTrue="1">
       <formula>AND($C42="Med Risk",L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="455" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="455" stopIfTrue="1">
       <formula>AND(LEN($C42)=0,L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:BO25">
-    <cfRule type="expression" dxfId="4" priority="486" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="486" stopIfTrue="1">
       <formula>AND($C27="Low Risk",L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="487" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="487" stopIfTrue="1">
       <formula>AND($C27="High Risk",L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="488" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="488" stopIfTrue="1">
       <formula>AND($C27="On Track",L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="489" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="489" stopIfTrue="1">
       <formula>AND($C27="Med Risk",L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="490" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="490" stopIfTrue="1">
       <formula>AND(LEN($C27)=0,L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8712,7 +8795,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>L35:BO37 L10:BO11 L8:BO8 L13:BO13 L31:BO32 L17:BO20</xm:sqref>
+          <xm:sqref>L35:BO37 L10:BO11 L8:BO8 L13:BO13 L31:BO32 L17:BO19 M20:BO20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="63" id="{51D83373-D7AE-4D2C-96F5-5741546F32FD}">

</xml_diff>

<commit_message>
หน้า add department role and หน้าaddCombobox
</commit_message>
<xml_diff>
--- a/20191118-Plan-Project-HR-Admin.xlsx
+++ b/20191118-Plan-Project-HR-Admin.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE23313-8D52-45A2-82A3-9B2E78769206}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778F7924-4157-4FE7-B198-A1367144DAC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
   <si>
     <t>About This Template</t>
   </si>
@@ -245,36 +245,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">4.1.2 Employee master                            </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">       *เหลือ import export</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4.2.1 Attendance                                 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*เหลือ การลาแบบไม่เต็มวัน</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">4.2.2 Date attendance                  </t>
     </r>
     <r>
@@ -317,6 +287,36 @@
       </rPr>
       <t xml:space="preserve">                                       *เหลือ filter</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.1.2 Employee master                            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                  *เหลือ import </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">4.2.1 Attendance                               </t>
+  </si>
+  <si>
+    <t>4.3 หน้า master เอาไว้ add data</t>
+  </si>
+  <si>
+    <t>4.3.2 master ของ combobox ทั้งหมด</t>
+  </si>
+  <si>
+    <t>4.3.1 master ของ department role</t>
+  </si>
+  <si>
+    <t>4.3.3 master ของ role การเข้าใช้งานระบบ</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,8 +574,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1080,6 +1086,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1108,7 +1134,7 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1596,6 +1622,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="11" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="11" borderId="43" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="11" borderId="43" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="19" fillId="11" borderId="43" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="12" borderId="16" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1614,272 +1664,6 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="72">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <sz val="10"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2820,6 +2604,272 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3130,20 +3180,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Milestones" displayName="Milestones" ref="B7:K41" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Milestones" displayName="Milestones" ref="B7:K45" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task Name" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Priority" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="%Progress" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start Date" dataDxfId="5" dataCellStyle="Date"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="End Date" dataDxfId="4" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Durations" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complete Date" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Delay" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task Name" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Priority" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="%Progress" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start Date" dataDxfId="52" dataCellStyle="Date"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="End Date" dataDxfId="51" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Durations" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complete Date" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Delay" dataDxfId="48">
       <calculatedColumnFormula>IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I8-Milestones[[#This Row],[End Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{95D18194-25A8-4EDA-B381-D3500AC79722}" name="Status" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{95D18194-25A8-4EDA-B381-D3500AC79722}" name="Status" dataDxfId="47">
       <calculatedColumnFormula>IF(Today=Milestones[[#This Row],[Start Date]],"On Process",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process","Complete")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3422,10 +3472,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO43"/>
+  <dimension ref="A1:BO47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5836,12 +5886,12 @@
         <v>43800</v>
       </c>
       <c r="G17" s="75">
-        <f>G29</f>
-        <v>43838</v>
+        <f>G34</f>
+        <v>43848</v>
       </c>
       <c r="H17" s="74">
-        <f>SUM(H19:H29)</f>
-        <v>38</v>
+        <f>SUM(H19:H34)</f>
+        <v>48</v>
       </c>
       <c r="I17" s="67"/>
       <c r="J17" s="69"/>
@@ -6236,7 +6286,7 @@
     <row r="20" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="78" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C20" s="65" t="s">
         <v>6</v>
@@ -6261,7 +6311,7 @@
       <c r="I20" s="151"/>
       <c r="J20" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],L20-Milestones[[#This Row],[End Date]])</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K20" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(L20-G20&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -6853,14 +6903,14 @@
     <row r="27" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="78" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C27" s="65"/>
       <c r="D27" s="65" t="s">
         <v>54</v>
       </c>
       <c r="E27" s="83">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F27" s="84">
         <f>G25</f>
@@ -6873,14 +6923,16 @@
       <c r="H27" s="73">
         <v>5</v>
       </c>
-      <c r="I27" s="84"/>
+      <c r="I27" s="84">
+        <v>43840</v>
+      </c>
       <c r="J27" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I27-Milestones[[#This Row],[End Date]])</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K27" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I27-G27&gt;0,"Delay","Complete"))),"Complete")</f>
-        <v>On Process</v>
+        <v>Complete</v>
       </c>
       <c r="L27" s="35"/>
       <c r="M27" s="10"/>
@@ -6942,7 +6994,7 @@
     <row r="28" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="78" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" s="65"/>
       <c r="D28" s="65" t="s">
@@ -6965,7 +7017,7 @@
       <c r="I28" s="84"/>
       <c r="J28" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I28-Milestones[[#This Row],[End Date]])</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K28" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I28-G28&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7030,7 +7082,7 @@
     </row>
     <row r="29" spans="1:67" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="78" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" s="65"/>
       <c r="D29" s="65" t="s">
@@ -7053,7 +7105,7 @@
       <c r="I29" s="84"/>
       <c r="J29" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I29-Milestones[[#This Row],[End Date]])</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K29" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I29-G29&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -7117,33 +7169,33 @@
       <c r="BO29" s="10"/>
     </row>
     <row r="30" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65" t="s">
+      <c r="B30" s="111" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="83">
+      <c r="E30" s="148">
         <v>0.9</v>
       </c>
-      <c r="F30" s="84">
+      <c r="F30" s="149">
         <f t="shared" si="15"/>
         <v>43838</v>
       </c>
-      <c r="G30" s="84">
+      <c r="G30" s="149">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
         <v>43843</v>
       </c>
-      <c r="H30" s="73">
+      <c r="H30" s="82">
         <v>5</v>
       </c>
-      <c r="I30" s="84"/>
-      <c r="J30" s="71">
+      <c r="I30" s="149"/>
+      <c r="J30" s="106">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I30-Milestones[[#This Row],[End Date]])</f>
-        <v>-5</v>
-      </c>
-      <c r="K30" s="71" t="str">
+        <v>0</v>
+      </c>
+      <c r="K30" s="106" t="str">
         <f ca="1">IF(Today=Milestones[[#This Row],[Start Date]],"On Process",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process","Complete")))</f>
         <v>On Process</v>
       </c>
@@ -7205,31 +7257,19 @@
       <c r="BO30" s="10"/>
     </row>
     <row r="31" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="95" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="92"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="56">
-        <f>G30</f>
-        <v>43843</v>
-      </c>
-      <c r="G31" s="56">
-        <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43849</v>
-      </c>
-      <c r="H31" s="134">
-        <f>H32</f>
-        <v>6</v>
-      </c>
-      <c r="I31" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="J31" s="98"/>
-      <c r="K31" s="98"/>
-      <c r="L31" s="108"/>
+      <c r="B31" s="165" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="166"/>
+      <c r="D31" s="166"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="168"/>
+      <c r="G31" s="169"/>
+      <c r="H31" s="170"/>
+      <c r="I31" s="168"/>
+      <c r="J31" s="171"/>
+      <c r="K31" s="171"/>
+      <c r="L31" s="35"/>
       <c r="M31" s="35"/>
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
@@ -7287,40 +7327,39 @@
       <c r="BO31" s="10"/>
     </row>
     <row r="32" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
-      <c r="B32" s="104" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="90" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="65" t="s">
+      <c r="B32" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="65"/>
+      <c r="D32" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="81">
-        <v>0</v>
-      </c>
-      <c r="F32" s="80">
-        <f>F31</f>
+      <c r="E32" s="83">
+        <v>1</v>
+      </c>
+      <c r="F32" s="84">
+        <f>G30</f>
         <v>43843</v>
       </c>
-      <c r="G32" s="80">
+      <c r="G32" s="84">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43849</v>
-      </c>
-      <c r="H32" s="82">
-        <v>6</v>
-      </c>
-      <c r="I32" s="105"/>
+        <v>43844</v>
+      </c>
+      <c r="H32" s="73">
+        <v>1</v>
+      </c>
+      <c r="I32" s="172">
+        <v>43843</v>
+      </c>
       <c r="J32" s="106">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I32-Milestones[[#This Row],[End Date]])</f>
-        <v>-11</v>
+        <v>-1</v>
       </c>
       <c r="K32" s="106" t="str">
-        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I32-G32&gt;0,"Delay","Complete"))),"Complete")</f>
-        <v>Pending</v>
-      </c>
-      <c r="L32" s="108"/>
+        <f ca="1">IF(Today=Milestones[[#This Row],[Start Date]],"On Process",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process","Complete")))</f>
+        <v>On Process</v>
+      </c>
+      <c r="L32" s="35"/>
       <c r="M32" s="35"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
@@ -7378,29 +7417,37 @@
       <c r="BO32" s="10"/>
     </row>
     <row r="33" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
-      <c r="B33" s="107" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="100"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="102"/>
-      <c r="F33" s="103">
-        <f>G32</f>
-        <v>43849</v>
-      </c>
-      <c r="G33" s="103">
+      <c r="B33" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="65"/>
+      <c r="D33" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="83">
+        <v>0</v>
+      </c>
+      <c r="F33" s="84">
+        <f t="shared" ref="F33:F34" si="16">G32</f>
+        <v>43844</v>
+      </c>
+      <c r="G33" s="84">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43855</v>
-      </c>
-      <c r="H33" s="86">
-        <f>H34</f>
-        <v>6</v>
-      </c>
-      <c r="I33" s="85"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="108"/>
+        <v>43846</v>
+      </c>
+      <c r="H33" s="73">
+        <v>2</v>
+      </c>
+      <c r="I33" s="172"/>
+      <c r="J33" s="106">
+        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I33-Milestones[[#This Row],[End Date]])</f>
+        <v>-3</v>
+      </c>
+      <c r="K33" s="106" t="str">
+        <f ca="1">IF(Today=Milestones[[#This Row],[Start Date]],"On Process",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process","Complete")))</f>
+        <v>Pending</v>
+      </c>
+      <c r="L33" s="35"/>
       <c r="M33" s="35"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
@@ -7458,39 +7505,37 @@
       <c r="BO33" s="10"/>
     </row>
     <row r="34" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="65" t="s">
+      <c r="B34" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="65"/>
+      <c r="D34" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="83">
         <v>0</v>
       </c>
-      <c r="F34" s="55">
-        <f>F33</f>
-        <v>43849</v>
-      </c>
-      <c r="G34" s="55">
+      <c r="F34" s="84">
+        <f t="shared" si="16"/>
+        <v>43846</v>
+      </c>
+      <c r="G34" s="84">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43855</v>
-      </c>
-      <c r="H34" s="87">
-        <v>6</v>
-      </c>
-      <c r="I34" s="99"/>
-      <c r="J34" s="70">
+        <v>43848</v>
+      </c>
+      <c r="H34" s="73">
+        <v>2</v>
+      </c>
+      <c r="I34" s="172"/>
+      <c r="J34" s="106">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I34-Milestones[[#This Row],[End Date]])</f>
-        <v>-17</v>
-      </c>
-      <c r="K34" s="70" t="str">
-        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I34-G34&gt;0,"Delay","Complete"))),"Complete")</f>
+        <v>-5</v>
+      </c>
+      <c r="K34" s="106" t="str">
+        <f ca="1">IF(Today=Milestones[[#This Row],[Start Date]],"On Process",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process","Complete")))</f>
         <v>Pending</v>
       </c>
-      <c r="L34" s="108"/>
+      <c r="L34" s="35"/>
       <c r="M34" s="35"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
@@ -7548,27 +7593,30 @@
       <c r="BO34" s="10"/>
     </row>
     <row r="35" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="100"/>
-      <c r="D35" s="101"/>
-      <c r="E35" s="102"/>
-      <c r="F35" s="103">
+      <c r="A35" s="42"/>
+      <c r="B35" s="95" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="92"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="56">
         <f>G34</f>
-        <v>43855</v>
-      </c>
-      <c r="G35" s="103">
+        <v>43848</v>
+      </c>
+      <c r="G35" s="56">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43861</v>
-      </c>
-      <c r="H35" s="86">
+        <v>43853</v>
+      </c>
+      <c r="H35" s="134">
         <f>H36</f>
-        <v>6</v>
-      </c>
-      <c r="I35" s="85"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
+        <v>5</v>
+      </c>
+      <c r="I35" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="98"/>
+      <c r="K35" s="98"/>
       <c r="L35" s="108"/>
       <c r="M35" s="35"/>
       <c r="N35" s="10"/>
@@ -7627,35 +7675,36 @@
       <c r="BO35" s="10"/>
     </row>
     <row r="36" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="60" t="s">
+      <c r="A36" s="42"/>
+      <c r="B36" s="104" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="90" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="58">
+      <c r="E36" s="81">
         <v>0</v>
       </c>
-      <c r="F36" s="57">
+      <c r="F36" s="80">
         <f>F35</f>
-        <v>43855</v>
-      </c>
-      <c r="G36" s="57">
+        <v>43848</v>
+      </c>
+      <c r="G36" s="80">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43861</v>
-      </c>
-      <c r="H36" s="54">
-        <v>6</v>
-      </c>
-      <c r="I36" s="94"/>
-      <c r="J36" s="71">
+        <v>43853</v>
+      </c>
+      <c r="H36" s="82">
+        <v>5</v>
+      </c>
+      <c r="I36" s="105"/>
+      <c r="J36" s="106">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I36-Milestones[[#This Row],[End Date]])</f>
-        <v>-23</v>
-      </c>
-      <c r="K36" s="71" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K36" s="106" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I36-G36&gt;0,"Delay","Complete"))),"Complete")</f>
         <v>Pending</v>
       </c>
@@ -7717,27 +7766,28 @@
       <c r="BO36" s="10"/>
     </row>
     <row r="37" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="95" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="92"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="56">
+      <c r="A37" s="42"/>
+      <c r="B37" s="107" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="100"/>
+      <c r="D37" s="101"/>
+      <c r="E37" s="102"/>
+      <c r="F37" s="103">
         <f>G36</f>
-        <v>43861</v>
-      </c>
-      <c r="G37" s="56">
+        <v>43853</v>
+      </c>
+      <c r="G37" s="103">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43866</v>
-      </c>
-      <c r="H37" s="97">
+        <v>43859</v>
+      </c>
+      <c r="H37" s="86">
         <f>H38</f>
-        <v>5</v>
-      </c>
-      <c r="I37" s="68"/>
-      <c r="J37" s="98"/>
-      <c r="K37" s="98"/>
+        <v>6</v>
+      </c>
+      <c r="I37" s="85"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
       <c r="L37" s="108"/>
       <c r="M37" s="35"/>
       <c r="N37" s="10"/>
@@ -7796,35 +7846,35 @@
       <c r="BO37" s="10"/>
     </row>
     <row r="38" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="60" t="s">
+      <c r="B38" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="61" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="58">
+      <c r="E38" s="59">
         <v>0</v>
       </c>
-      <c r="F38" s="57">
+      <c r="F38" s="55">
         <f>F37</f>
-        <v>43861</v>
-      </c>
-      <c r="G38" s="57">
+        <v>43853</v>
+      </c>
+      <c r="G38" s="55">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43866</v>
-      </c>
-      <c r="H38" s="54">
-        <v>5</v>
-      </c>
-      <c r="I38" s="94"/>
-      <c r="J38" s="71">
+        <v>43859</v>
+      </c>
+      <c r="H38" s="87">
+        <v>6</v>
+      </c>
+      <c r="I38" s="99"/>
+      <c r="J38" s="70">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I38-Milestones[[#This Row],[End Date]])</f>
-        <v>-28</v>
-      </c>
-      <c r="K38" s="71" t="str">
+        <v>-16</v>
+      </c>
+      <c r="K38" s="70" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I38-G38&gt;0,"Delay","Complete"))),"Complete")</f>
         <v>Pending</v>
       </c>
@@ -7885,26 +7935,24 @@
       <c r="BN38" s="10"/>
       <c r="BO38" s="10"/>
     </row>
-    <row r="39" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="89" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="66"/>
-      <c r="E39" s="96"/>
-      <c r="F39" s="75">
+    <row r="39" spans="1:67" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="100"/>
+      <c r="D39" s="101"/>
+      <c r="E39" s="102"/>
+      <c r="F39" s="103">
         <f>G38</f>
-        <v>43866</v>
+        <v>43859</v>
       </c>
       <c r="G39" s="103">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43873</v>
+        <v>43865</v>
       </c>
       <c r="H39" s="86">
         <f>H40</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I39" s="85"/>
       <c r="J39" s="69"/>
@@ -7966,34 +8014,34 @@
       <c r="BN39" s="10"/>
       <c r="BO39" s="10"/>
     </row>
-    <row r="40" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="131" t="s">
+    <row r="40" spans="1:67" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="76" t="s">
+      <c r="D40" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="83">
+      <c r="E40" s="58">
         <v>0</v>
       </c>
       <c r="F40" s="57">
         <f>F39</f>
-        <v>43866</v>
+        <v>43859</v>
       </c>
       <c r="G40" s="57">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43873</v>
+        <v>43865</v>
       </c>
       <c r="H40" s="54">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I40" s="94"/>
       <c r="J40" s="71">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I40-Milestones[[#This Row],[End Date]])</f>
-        <v>-35</v>
+        <v>-22</v>
       </c>
       <c r="K40" s="71" t="str">
         <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I40-G40&gt;0,"Delay","Complete"))),"Complete")</f>
@@ -8056,38 +8104,29 @@
       <c r="BN40" s="10"/>
       <c r="BO40" s="10"/>
     </row>
-    <row r="41" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="78" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="65"/>
-      <c r="D41" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="118">
-        <v>0</v>
-      </c>
-      <c r="F41" s="55">
+    <row r="41" spans="1:67" ht="15" x14ac:dyDescent="0.25">
+      <c r="B41" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="92"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="56">
         <f>G40</f>
-        <v>43873</v>
-      </c>
-      <c r="G41" s="55">
+        <v>43865</v>
+      </c>
+      <c r="G41" s="56">
         <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
-        <v>43880</v>
-      </c>
-      <c r="H41" s="87">
-        <v>7</v>
-      </c>
-      <c r="I41" s="99"/>
-      <c r="J41" s="70">
-        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I41-Milestones[[#This Row],[End Date]])</f>
-        <v>-42</v>
-      </c>
-      <c r="K41" s="70" t="str">
-        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I41-G41&gt;0,"Delay","Complete"))),"Complete")</f>
-        <v>Pending</v>
-      </c>
-      <c r="L41" s="35"/>
+        <v>43866</v>
+      </c>
+      <c r="H41" s="97">
+        <f>H42</f>
+        <v>1</v>
+      </c>
+      <c r="I41" s="68"/>
+      <c r="J41" s="98"/>
+      <c r="K41" s="98"/>
+      <c r="L41" s="108"/>
       <c r="M41" s="35"/>
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
@@ -8144,11 +8183,360 @@
       <c r="BN41" s="10"/>
       <c r="BO41" s="10"/>
     </row>
-    <row r="42" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="30"/>
+    <row r="42" spans="1:67" ht="15" x14ac:dyDescent="0.25">
+      <c r="B42" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="58">
+        <v>0</v>
+      </c>
+      <c r="F42" s="57">
+        <f>F41</f>
+        <v>43865</v>
+      </c>
+      <c r="G42" s="57">
+        <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
+        <v>43866</v>
+      </c>
+      <c r="H42" s="54">
+        <v>1</v>
+      </c>
+      <c r="I42" s="94"/>
+      <c r="J42" s="71">
+        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I42-Milestones[[#This Row],[End Date]])</f>
+        <v>-23</v>
+      </c>
+      <c r="K42" s="71" t="str">
+        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I42-G42&gt;0,"Delay","Complete"))),"Complete")</f>
+        <v>Pending</v>
+      </c>
+      <c r="L42" s="108"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="10"/>
+      <c r="AB42" s="10"/>
+      <c r="AC42" s="10"/>
+      <c r="AD42" s="10"/>
+      <c r="AE42" s="10"/>
+      <c r="AF42" s="10"/>
+      <c r="AG42" s="10"/>
+      <c r="AH42" s="10"/>
+      <c r="AI42" s="10"/>
+      <c r="AJ42" s="10"/>
+      <c r="AK42" s="10"/>
+      <c r="AL42" s="10"/>
+      <c r="AM42" s="10"/>
+      <c r="AN42" s="10"/>
+      <c r="AO42" s="10"/>
+      <c r="AP42" s="10"/>
+      <c r="AQ42" s="10"/>
+      <c r="AR42" s="10"/>
+      <c r="AS42" s="10"/>
+      <c r="AT42" s="10"/>
+      <c r="AU42" s="10"/>
+      <c r="AV42" s="10"/>
+      <c r="AW42" s="10"/>
+      <c r="AX42" s="10"/>
+      <c r="AY42" s="10"/>
+      <c r="AZ42" s="10"/>
+      <c r="BA42" s="10"/>
+      <c r="BB42" s="10"/>
+      <c r="BC42" s="10"/>
+      <c r="BD42" s="10"/>
+      <c r="BE42" s="10"/>
+      <c r="BF42" s="10"/>
+      <c r="BG42" s="10"/>
+      <c r="BH42" s="10"/>
+      <c r="BI42" s="10"/>
+      <c r="BJ42" s="10"/>
+      <c r="BK42" s="10"/>
+      <c r="BL42" s="10"/>
+      <c r="BM42" s="10"/>
+      <c r="BN42" s="10"/>
+      <c r="BO42" s="10"/>
     </row>
-    <row r="43" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D43" s="30"/>
+    <row r="43" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="89" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="66"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="75">
+        <f>G42</f>
+        <v>43866</v>
+      </c>
+      <c r="G43" s="103">
+        <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
+        <v>43873</v>
+      </c>
+      <c r="H43" s="86">
+        <f>H44</f>
+        <v>7</v>
+      </c>
+      <c r="I43" s="85"/>
+      <c r="J43" s="69"/>
+      <c r="K43" s="69"/>
+      <c r="L43" s="108"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10"/>
+      <c r="W43" s="10"/>
+      <c r="X43" s="10"/>
+      <c r="Y43" s="10"/>
+      <c r="Z43" s="10"/>
+      <c r="AA43" s="10"/>
+      <c r="AB43" s="10"/>
+      <c r="AC43" s="10"/>
+      <c r="AD43" s="10"/>
+      <c r="AE43" s="10"/>
+      <c r="AF43" s="10"/>
+      <c r="AG43" s="10"/>
+      <c r="AH43" s="10"/>
+      <c r="AI43" s="10"/>
+      <c r="AJ43" s="10"/>
+      <c r="AK43" s="10"/>
+      <c r="AL43" s="10"/>
+      <c r="AM43" s="10"/>
+      <c r="AN43" s="10"/>
+      <c r="AO43" s="10"/>
+      <c r="AP43" s="10"/>
+      <c r="AQ43" s="10"/>
+      <c r="AR43" s="10"/>
+      <c r="AS43" s="10"/>
+      <c r="AT43" s="10"/>
+      <c r="AU43" s="10"/>
+      <c r="AV43" s="10"/>
+      <c r="AW43" s="10"/>
+      <c r="AX43" s="10"/>
+      <c r="AY43" s="10"/>
+      <c r="AZ43" s="10"/>
+      <c r="BA43" s="10"/>
+      <c r="BB43" s="10"/>
+      <c r="BC43" s="10"/>
+      <c r="BD43" s="10"/>
+      <c r="BE43" s="10"/>
+      <c r="BF43" s="10"/>
+      <c r="BG43" s="10"/>
+      <c r="BH43" s="10"/>
+      <c r="BI43" s="10"/>
+      <c r="BJ43" s="10"/>
+      <c r="BK43" s="10"/>
+      <c r="BL43" s="10"/>
+      <c r="BM43" s="10"/>
+      <c r="BN43" s="10"/>
+      <c r="BO43" s="10"/>
+    </row>
+    <row r="44" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="131" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="83">
+        <v>0</v>
+      </c>
+      <c r="F44" s="57">
+        <f>F43</f>
+        <v>43866</v>
+      </c>
+      <c r="G44" s="57">
+        <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
+        <v>43873</v>
+      </c>
+      <c r="H44" s="54">
+        <v>7</v>
+      </c>
+      <c r="I44" s="94"/>
+      <c r="J44" s="71">
+        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I44-Milestones[[#This Row],[End Date]])</f>
+        <v>-30</v>
+      </c>
+      <c r="K44" s="71" t="str">
+        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I44-G44&gt;0,"Delay","Complete"))),"Complete")</f>
+        <v>Pending</v>
+      </c>
+      <c r="L44" s="108"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="10"/>
+      <c r="U44" s="10"/>
+      <c r="V44" s="10"/>
+      <c r="W44" s="10"/>
+      <c r="X44" s="10"/>
+      <c r="Y44" s="10"/>
+      <c r="Z44" s="10"/>
+      <c r="AA44" s="10"/>
+      <c r="AB44" s="10"/>
+      <c r="AC44" s="10"/>
+      <c r="AD44" s="10"/>
+      <c r="AE44" s="10"/>
+      <c r="AF44" s="10"/>
+      <c r="AG44" s="10"/>
+      <c r="AH44" s="10"/>
+      <c r="AI44" s="10"/>
+      <c r="AJ44" s="10"/>
+      <c r="AK44" s="10"/>
+      <c r="AL44" s="10"/>
+      <c r="AM44" s="10"/>
+      <c r="AN44" s="10"/>
+      <c r="AO44" s="10"/>
+      <c r="AP44" s="10"/>
+      <c r="AQ44" s="10"/>
+      <c r="AR44" s="10"/>
+      <c r="AS44" s="10"/>
+      <c r="AT44" s="10"/>
+      <c r="AU44" s="10"/>
+      <c r="AV44" s="10"/>
+      <c r="AW44" s="10"/>
+      <c r="AX44" s="10"/>
+      <c r="AY44" s="10"/>
+      <c r="AZ44" s="10"/>
+      <c r="BA44" s="10"/>
+      <c r="BB44" s="10"/>
+      <c r="BC44" s="10"/>
+      <c r="BD44" s="10"/>
+      <c r="BE44" s="10"/>
+      <c r="BF44" s="10"/>
+      <c r="BG44" s="10"/>
+      <c r="BH44" s="10"/>
+      <c r="BI44" s="10"/>
+      <c r="BJ44" s="10"/>
+      <c r="BK44" s="10"/>
+      <c r="BL44" s="10"/>
+      <c r="BM44" s="10"/>
+      <c r="BN44" s="10"/>
+      <c r="BO44" s="10"/>
+    </row>
+    <row r="45" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" s="118">
+        <v>0</v>
+      </c>
+      <c r="F45" s="55">
+        <f>G44</f>
+        <v>43873</v>
+      </c>
+      <c r="G45" s="55">
+        <f>Milestones[[#This Row],[Start Date]]+Milestones[[#This Row],[Durations]]</f>
+        <v>43880</v>
+      </c>
+      <c r="H45" s="87">
+        <v>7</v>
+      </c>
+      <c r="I45" s="99"/>
+      <c r="J45" s="70">
+        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",TODAY()-Milestones[[#This Row],[End Date]],I45-Milestones[[#This Row],[End Date]])</f>
+        <v>-37</v>
+      </c>
+      <c r="K45" s="70" t="str">
+        <f ca="1">IF(Milestones[[#This Row],[Complete Date]]="",IF(TODAY()&lt;Milestones[[#This Row],[Start Date]],"Pending",IF(Milestones[[#This Row],[Complete Date]]="","On Process",IF(I45-G45&gt;0,"Delay","Complete"))),"Complete")</f>
+        <v>Pending</v>
+      </c>
+      <c r="L45" s="35"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="10"/>
+      <c r="V45" s="10"/>
+      <c r="W45" s="10"/>
+      <c r="X45" s="10"/>
+      <c r="Y45" s="10"/>
+      <c r="Z45" s="10"/>
+      <c r="AA45" s="10"/>
+      <c r="AB45" s="10"/>
+      <c r="AC45" s="10"/>
+      <c r="AD45" s="10"/>
+      <c r="AE45" s="10"/>
+      <c r="AF45" s="10"/>
+      <c r="AG45" s="10"/>
+      <c r="AH45" s="10"/>
+      <c r="AI45" s="10"/>
+      <c r="AJ45" s="10"/>
+      <c r="AK45" s="10"/>
+      <c r="AL45" s="10"/>
+      <c r="AM45" s="10"/>
+      <c r="AN45" s="10"/>
+      <c r="AO45" s="10"/>
+      <c r="AP45" s="10"/>
+      <c r="AQ45" s="10"/>
+      <c r="AR45" s="10"/>
+      <c r="AS45" s="10"/>
+      <c r="AT45" s="10"/>
+      <c r="AU45" s="10"/>
+      <c r="AV45" s="10"/>
+      <c r="AW45" s="10"/>
+      <c r="AX45" s="10"/>
+      <c r="AY45" s="10"/>
+      <c r="AZ45" s="10"/>
+      <c r="BA45" s="10"/>
+      <c r="BB45" s="10"/>
+      <c r="BC45" s="10"/>
+      <c r="BD45" s="10"/>
+      <c r="BE45" s="10"/>
+      <c r="BF45" s="10"/>
+      <c r="BG45" s="10"/>
+      <c r="BH45" s="10"/>
+      <c r="BI45" s="10"/>
+      <c r="BJ45" s="10"/>
+      <c r="BK45" s="10"/>
+      <c r="BL45" s="10"/>
+      <c r="BM45" s="10"/>
+      <c r="BN45" s="10"/>
+      <c r="BO45" s="10"/>
+    </row>
+    <row r="46" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="30"/>
+    </row>
+    <row r="47" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -8162,7 +8550,7 @@
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="V2:Y2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:E8 E10:E11 E37 E39 E13 E33 E17:E31">
+  <conditionalFormatting sqref="E7:E8 E10:E11 E41 E43 E13 E37 E17:E35">
     <cfRule type="dataBar" priority="160">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8176,40 +8564,40 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5:BO8 L10:BO11 L35:BO37 L13:BO13 L17:BO20 L31:BO32">
-    <cfRule type="expression" dxfId="59" priority="153">
+  <conditionalFormatting sqref="L5:BO8 L10:BO11 L39:BO41 L13:BO13 L17:BO20 L35:BO36">
+    <cfRule type="expression" dxfId="46" priority="153">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:AP4">
-    <cfRule type="expression" dxfId="58" priority="159">
+    <cfRule type="expression" dxfId="45" priority="159">
       <formula>L$5&lt;=EOMONTH($L$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:BO4">
-    <cfRule type="expression" dxfId="57" priority="155">
+    <cfRule type="expression" dxfId="44" priority="155">
       <formula>AND(M$5&lt;=EOMONTH($L$5,2),M$5&gt;EOMONTH($L$5,0),M$5&gt;EOMONTH($L$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:BO4">
-    <cfRule type="expression" dxfId="56" priority="154">
+    <cfRule type="expression" dxfId="43" priority="154">
       <formula>AND(L$5&lt;=EOMONTH($L$5,1),L$5&gt;EOMONTH($L$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:BO17">
-    <cfRule type="expression" dxfId="55" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="176" stopIfTrue="1">
       <formula>AND($C8="Low Risk",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="195" stopIfTrue="1">
       <formula>AND($C8="High Risk",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="213" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="213" stopIfTrue="1">
       <formula>AND($C8="On Track",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="214" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="214" stopIfTrue="1">
       <formula>AND($C8="Med Risk",L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="215" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="215" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,L$5&gt;=$F8,L$5&lt;=$F8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8228,7 +8616,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:BO12">
-    <cfRule type="expression" dxfId="50" priority="128">
+    <cfRule type="expression" dxfId="37" priority="128">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8247,16 +8635,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:BO9">
-    <cfRule type="expression" dxfId="49" priority="120">
+    <cfRule type="expression" dxfId="36" priority="120">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L34:BO37">
-    <cfRule type="expression" dxfId="48" priority="64">
+  <conditionalFormatting sqref="L38:BO41">
+    <cfRule type="expression" dxfId="35" priority="64">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37 E39">
+  <conditionalFormatting sqref="E41 E43">
     <cfRule type="dataBar" priority="65">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8270,23 +8658,23 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L38:BO38">
-    <cfRule type="expression" dxfId="47" priority="56">
+  <conditionalFormatting sqref="L42:BO42">
+    <cfRule type="expression" dxfId="34" priority="56">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L38:BO38">
-    <cfRule type="expression" dxfId="46" priority="54">
+  <conditionalFormatting sqref="L42:BO42">
+    <cfRule type="expression" dxfId="33" priority="54">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L21:BO30">
-    <cfRule type="expression" dxfId="45" priority="43">
+  <conditionalFormatting sqref="L21:BO34">
+    <cfRule type="expression" dxfId="32" priority="43">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:BO15">
-    <cfRule type="expression" dxfId="44" priority="33">
+    <cfRule type="expression" dxfId="31" priority="33">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8305,11 +8693,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:BO16 L14:BO14">
-    <cfRule type="expression" dxfId="43" priority="35">
+    <cfRule type="expression" dxfId="30" priority="35">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E36">
     <cfRule type="dataBar" priority="32">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8323,7 +8711,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
+  <conditionalFormatting sqref="E38">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8337,7 +8725,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+  <conditionalFormatting sqref="E40">
     <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8351,7 +8739,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
+  <conditionalFormatting sqref="E42">
     <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8365,7 +8753,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40:E41">
+  <conditionalFormatting sqref="E44:E45">
     <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8379,7 +8767,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
+  <conditionalFormatting sqref="E39">
     <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8393,113 +8781,113 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L33:BO33">
-    <cfRule type="expression" dxfId="42" priority="18">
+  <conditionalFormatting sqref="L37:BO37">
+    <cfRule type="expression" dxfId="29" priority="18">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:BO19 L21:BO21 M20:BO20">
-    <cfRule type="expression" dxfId="41" priority="409" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="409" stopIfTrue="1">
       <formula>AND($C19="Low Risk",L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="410" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="410" stopIfTrue="1">
       <formula>AND($C19="High Risk",L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="411" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="411" stopIfTrue="1">
       <formula>AND($C19="On Track",L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="412" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="412" stopIfTrue="1">
       <formula>AND($C19="Med Risk",L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="413" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="413" stopIfTrue="1">
       <formula>AND(LEN($C19)=0,L$5&gt;=$F19,L$5&lt;=$F19+$H19-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L26:BO27 L31:BO38">
-    <cfRule type="expression" dxfId="36" priority="421" stopIfTrue="1">
+  <conditionalFormatting sqref="L26:BO27 L35:BO42">
+    <cfRule type="expression" dxfId="23" priority="421" stopIfTrue="1">
       <formula>AND($C28="Low Risk",L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="422" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="422" stopIfTrue="1">
       <formula>AND($C28="High Risk",L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="423" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="423" stopIfTrue="1">
       <formula>AND($C28="On Track",L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="424" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="424" stopIfTrue="1">
       <formula>AND($C28="Med Risk",L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="425" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="425" stopIfTrue="1">
       <formula>AND(LEN($C28)=0,L$5&gt;=$F28,L$5&lt;=$F28+$H28-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L28:BO30">
-    <cfRule type="expression" dxfId="31" priority="445" stopIfTrue="1">
+  <conditionalFormatting sqref="L28:BO34">
+    <cfRule type="expression" dxfId="18" priority="445" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="446" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="446" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="447" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="447" stopIfTrue="1">
       <formula>AND(#REF!="On Track",L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="448" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="448" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="449" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="449" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,L$5&gt;=#REF!,L$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L39:BO39">
-    <cfRule type="expression" dxfId="26" priority="11">
+  <conditionalFormatting sqref="L43:BO43">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L39:BO39">
-    <cfRule type="expression" dxfId="25" priority="10">
+  <conditionalFormatting sqref="L43:BO43">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40:BO41">
-    <cfRule type="expression" dxfId="24" priority="3">
+  <conditionalFormatting sqref="L44:BO45">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40:BO41">
-    <cfRule type="expression" dxfId="23" priority="2">
+  <conditionalFormatting sqref="L44:BO45">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L39:BO41">
-    <cfRule type="expression" dxfId="22" priority="451" stopIfTrue="1">
-      <formula>AND($C42="Low Risk",L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
+  <conditionalFormatting sqref="L43:BO45">
+    <cfRule type="expression" dxfId="9" priority="451" stopIfTrue="1">
+      <formula>AND($C46="Low Risk",L$5&gt;=$F46,L$5&lt;=$F46+$H46-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="452" stopIfTrue="1">
-      <formula>AND($C42="High Risk",L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
+    <cfRule type="expression" dxfId="8" priority="452" stopIfTrue="1">
+      <formula>AND($C46="High Risk",L$5&gt;=$F46,L$5&lt;=$F46+$H46-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="453" stopIfTrue="1">
-      <formula>AND($C42="On Track",L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
+    <cfRule type="expression" dxfId="7" priority="453" stopIfTrue="1">
+      <formula>AND($C46="On Track",L$5&gt;=$F46,L$5&lt;=$F46+$H46-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="454" stopIfTrue="1">
-      <formula>AND($C42="Med Risk",L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
+    <cfRule type="expression" dxfId="6" priority="454" stopIfTrue="1">
+      <formula>AND($C46="Med Risk",L$5&gt;=$F46,L$5&lt;=$F46+$H46-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="455" stopIfTrue="1">
-      <formula>AND(LEN($C42)=0,L$5&gt;=$F42,L$5&lt;=$F42+$H42-1)</formula>
+    <cfRule type="expression" dxfId="5" priority="455" stopIfTrue="1">
+      <formula>AND(LEN($C46)=0,L$5&gt;=$F46,L$5&lt;=$F46+$H46-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:BO25">
-    <cfRule type="expression" dxfId="17" priority="486" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="486" stopIfTrue="1">
       <formula>AND($C27="Low Risk",L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="487" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="487" stopIfTrue="1">
       <formula>AND($C27="High Risk",L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="488" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="488" stopIfTrue="1">
       <formula>AND($C27="On Track",L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="489" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="489" stopIfTrue="1">
       <formula>AND($C27="Med Risk",L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="490" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="490" stopIfTrue="1">
       <formula>AND(LEN($C27)=0,L$5&gt;=$F27,L$5&lt;=$F27+$H27-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8507,7 +8895,7 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4:G4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C41" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C45" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8518,7 +8906,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F32" formula="1"/>
+    <ignoredError sqref="F36" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -8569,7 +8957,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E7:E8 E10:E11 E37 E39 E13 E33 E17:E31</xm:sqref>
+          <xm:sqref>E7:E8 E10:E11 E41 E43 E13 E37 E17:E35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3450C8A0-7296-4F4E-8C2D-67F62EE92A11}">
@@ -8614,7 +9002,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E37 E39</xm:sqref>
+          <xm:sqref>E41 E43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{204492DB-C9DC-4A29-B7D2-317B3BB60E18}">
@@ -8644,7 +9032,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E32</xm:sqref>
+          <xm:sqref>E36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7D6D8DC0-8DB6-471B-8654-216B06E96310}">
@@ -8659,7 +9047,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E34</xm:sqref>
+          <xm:sqref>E38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{72B44424-0899-4A95-A18C-814AFD22EEB5}">
@@ -8674,7 +9062,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E36</xm:sqref>
+          <xm:sqref>E40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6E8DB8E0-4C2B-4E51-A644-0734E8A3FFDF}">
@@ -8689,7 +9077,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E38</xm:sqref>
+          <xm:sqref>E42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{29A332D1-8F3D-4822-AAE4-11C27860126D}">
@@ -8704,7 +9092,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E40:E41</xm:sqref>
+          <xm:sqref>E44:E45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{08AC8ABD-7BBE-46E4-88DE-E740474021EA}">
@@ -8719,7 +9107,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E35</xm:sqref>
+          <xm:sqref>E39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="135" id="{C6DA3BC1-C08C-46A6-9965-548C4725E846}">
@@ -8776,7 +9164,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>L34:BO34</xm:sqref>
+          <xm:sqref>L38:BO38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="401" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
@@ -8795,7 +9183,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>L35:BO37 L10:BO11 L8:BO8 L13:BO13 L31:BO32 L17:BO19 M20:BO20</xm:sqref>
+          <xm:sqref>L39:BO41 L10:BO11 L8:BO8 L13:BO13 L35:BO36 L17:BO19 M20:BO20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="63" id="{51D83373-D7AE-4D2C-96F5-5741546F32FD}">
@@ -8814,7 +9202,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>L38:BO38</xm:sqref>
+          <xm:sqref>L42:BO42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="34" id="{22963F08-ED33-4A2E-B7DC-CED3CC34C068}">
@@ -8871,7 +9259,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>L33:BO33</xm:sqref>
+          <xm:sqref>L37:BO37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="434" id="{21FC89A8-1110-4FE8-AE4F-B89BB56E6A72}">
@@ -8890,7 +9278,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>L21:BO30</xm:sqref>
+          <xm:sqref>L21:BO34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{B2096DA8-8ECA-47CE-B1DF-8F1E2E08633E}">
@@ -8909,7 +9297,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>L39:BO39</xm:sqref>
+          <xm:sqref>L43:BO43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="4" id="{98A44775-E807-4593-914E-8823CF8761D4}">
@@ -8928,7 +9316,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>L40:BO41</xm:sqref>
+          <xm:sqref>L44:BO45</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>